<commit_message>
Updating code for 2023 workup. New code includes: - considerations for adding weight to a variety of SPC without lenwt regressions. - for any species with biocnt = catcnt the actual weights were used
</commit_message>
<xml_diff>
--- a/Data/Groups_1.xlsx
+++ b/Data/Groups_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ontariogov-my.sharepoint.com/personal/sarah_beech1_ontario_ca/Documents/Documents/R projects/NSCIN2022/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ontariogov-my.sharepoint.com/personal/alex_row_ontario_ca/Documents/Desktop/NSCIN 2023/R/NSCIN_R_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="11_10724789CA3B95BB80201810700B18B80BB9EDAA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DB5DC0A-DFB0-4203-A59B-62267C4F0159}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{54D3FEAC-C0BD-44F8-A9FD-779390092309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Groups_1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1238" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1273" uniqueCount="19">
   <si>
     <t>SPC</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Musy/pike are categorised different for warm/cool water - unsure where to categorise</t>
   </si>
 </sst>
 </file>
@@ -571,9 +574,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -895,10 +899,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P95"/>
+  <dimension ref="A1:Q98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N97" sqref="N97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5671,7 +5676,131 @@
         <v>17</v>
       </c>
     </row>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>483</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G96" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H96" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I96" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J96" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L96" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N96" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O96" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P96" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>502</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H97" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I97" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J97" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K97" s="1">
+        <v>1</v>
+      </c>
+      <c r="L97" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P97" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q97" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>213</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H98" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I98" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J98" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L98" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated file to incldue information on yellow bullhead. I used the identical information from brown bullhead
</commit_message>
<xml_diff>
--- a/Data/Groups_1.xlsx
+++ b/Data/Groups_1.xlsx
@@ -5,18 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ontariogov-my.sharepoint.com/personal/alex_row_ontario_ca/Documents/Desktop/NSCIN 2023/R/NSCIN_R_2023/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ontariogov-my.sharepoint.com/personal/alex_row_ontario_ca/Documents/Desktop/NSCIN 2023/R/NSCIN_R_2023/NSCIN workup/NSCIN2023/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{54D3FEAC-C0BD-44F8-A9FD-779390092309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{54D3FEAC-C0BD-44F8-A9FD-779390092309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05D54561-DC46-4D45-A259-E2943BCD8B13}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24120" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Groups_1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Database">Groups_1!$A$1:$P$95</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Groups_1!$A$1:$A$99</definedName>
+    <definedName name="_xlnm.Database">Groups_1!$A$1:$P$96</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1273" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1286" uniqueCount="19">
   <si>
     <t>SPC</t>
   </si>
@@ -899,11 +900,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q98"/>
+  <dimension ref="A1:Q99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N97" sqref="N97"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3828,7 +3829,7 @@
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>16</v>
@@ -3878,7 +3879,7 @@
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>16</v>
@@ -3928,7 +3929,7 @@
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>16</v>
@@ -3978,7 +3979,7 @@
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>16</v>
@@ -3993,7 +3994,7 @@
         <v>17</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>17</v>
@@ -4014,13 +4015,13 @@
         <v>16</v>
       </c>
       <c r="M62" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N62" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O62" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="P62" s="1" t="s">
         <v>17</v>
@@ -4028,7 +4029,7 @@
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>16</v>
@@ -4043,13 +4044,13 @@
         <v>17</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I63" s="1" t="s">
         <v>17</v>
@@ -4058,7 +4059,7 @@
         <v>17</v>
       </c>
       <c r="K63" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L63" s="1" t="s">
         <v>16</v>
@@ -4078,7 +4079,7 @@
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>16</v>
@@ -4096,19 +4097,19 @@
         <v>17</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H64" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J64" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K64" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L64" s="1" t="s">
         <v>16</v>
@@ -4128,7 +4129,7 @@
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>16</v>
@@ -4146,39 +4147,39 @@
         <v>17</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K65" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L65" s="1" t="s">
         <v>16</v>
       </c>
       <c r="M65" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N65" s="1" t="s">
         <v>17</v>
       </c>
       <c r="O65" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P65" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>16</v>
@@ -4196,39 +4197,39 @@
         <v>17</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K66" s="1">
+        <v>1</v>
+      </c>
+      <c r="L66" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M66" s="1">
         <v>3</v>
       </c>
-      <c r="L66" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M66" s="1">
-        <v>2</v>
-      </c>
       <c r="N66" s="1" t="s">
         <v>17</v>
       </c>
       <c r="O66" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="P66" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>16</v>
@@ -4278,7 +4279,7 @@
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>16</v>
@@ -4299,16 +4300,16 @@
         <v>17</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K68" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L68" s="1" t="s">
         <v>16</v>
@@ -4328,7 +4329,7 @@
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>16</v>
@@ -4349,42 +4350,42 @@
         <v>17</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K69" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L69" s="1" t="s">
         <v>16</v>
       </c>
       <c r="M69" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N69" s="1" t="s">
         <v>17</v>
       </c>
       <c r="O69" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P69" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>17</v>
@@ -4405,7 +4406,7 @@
         <v>16</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K70" s="1">
         <v>3</v>
@@ -4414,27 +4415,27 @@
         <v>16</v>
       </c>
       <c r="M70" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N70" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O70" s="1" t="s">
         <v>17</v>
       </c>
       <c r="P70" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>17</v>
@@ -4478,7 +4479,7 @@
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>16</v>
@@ -4528,7 +4529,7 @@
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>16</v>
@@ -4537,7 +4538,7 @@
         <v>17</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>17</v>
@@ -4555,7 +4556,7 @@
         <v>16</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K73" s="1">
         <v>3</v>
@@ -4578,7 +4579,7 @@
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>16</v>
@@ -4593,7 +4594,7 @@
         <v>17</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G74" s="1" t="s">
         <v>17</v>
@@ -4628,7 +4629,7 @@
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>16</v>
@@ -4643,7 +4644,7 @@
         <v>17</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G75" s="1" t="s">
         <v>17</v>
@@ -4678,7 +4679,7 @@
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>16</v>
@@ -4728,7 +4729,7 @@
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>16</v>
@@ -4778,7 +4779,7 @@
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>16</v>
@@ -4796,19 +4797,19 @@
         <v>17</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H78" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J78" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K78" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L78" s="1" t="s">
         <v>16</v>
@@ -4828,7 +4829,7 @@
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>16</v>
@@ -4878,7 +4879,7 @@
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>16</v>
@@ -4896,19 +4897,19 @@
         <v>17</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H80" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J80" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K80" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L80" s="1" t="s">
         <v>16</v>
@@ -4928,7 +4929,7 @@
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>16</v>
@@ -4978,7 +4979,7 @@
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>331</v>
+        <v>320</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>16</v>
@@ -4987,7 +4988,7 @@
         <v>17</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>17</v>
@@ -5014,13 +5015,13 @@
         <v>16</v>
       </c>
       <c r="M82" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N82" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O82" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="P82" s="1" t="s">
         <v>17</v>
@@ -5028,7 +5029,7 @@
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>16</v>
@@ -5046,19 +5047,19 @@
         <v>17</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H83" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J83" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K83" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L83" s="1" t="s">
         <v>16</v>
@@ -5078,7 +5079,7 @@
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>16</v>
@@ -5093,34 +5094,34 @@
         <v>17</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H84" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J84" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K84" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L84" s="1" t="s">
         <v>16</v>
       </c>
       <c r="M84" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N84" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O84" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P84" s="1" t="s">
         <v>17</v>
@@ -5128,7 +5129,7 @@
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>16</v>
@@ -5143,7 +5144,7 @@
         <v>17</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G85" s="1" t="s">
         <v>17</v>
@@ -5155,7 +5156,7 @@
         <v>16</v>
       </c>
       <c r="J85" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K85" s="1">
         <v>3</v>
@@ -5164,13 +5165,13 @@
         <v>16</v>
       </c>
       <c r="M85" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N85" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O85" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="P85" s="1" t="s">
         <v>17</v>
@@ -5178,7 +5179,7 @@
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>16</v>
@@ -5228,7 +5229,7 @@
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>16</v>
@@ -5278,7 +5279,7 @@
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>361</v>
+        <v>342</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>16</v>
@@ -5293,7 +5294,7 @@
         <v>17</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G88" s="1" t="s">
         <v>17</v>
@@ -5305,7 +5306,7 @@
         <v>16</v>
       </c>
       <c r="J88" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K88" s="1">
         <v>3</v>
@@ -5328,13 +5329,13 @@
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>17</v>
@@ -5343,22 +5344,22 @@
         <v>17</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G89" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J89" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K89" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L89" s="1" t="s">
         <v>16</v>
@@ -5378,7 +5379,7 @@
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>17</v>
@@ -5428,13 +5429,13 @@
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>17</v>
@@ -5449,28 +5450,28 @@
         <v>17</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J91" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K91" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L91" s="1" t="s">
         <v>16</v>
       </c>
       <c r="M91" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N91" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O91" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P91" s="1" t="s">
         <v>17</v>
@@ -5478,7 +5479,7 @@
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>382</v>
+        <v>371</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>16</v>
@@ -5514,21 +5515,21 @@
         <v>16</v>
       </c>
       <c r="M92" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N92" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O92" s="1" t="s">
         <v>17</v>
       </c>
       <c r="P92" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>16</v>
@@ -5549,42 +5550,42 @@
         <v>17</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J93" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K93" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L93" s="1" t="s">
         <v>16</v>
       </c>
       <c r="M93" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N93" s="1" t="s">
         <v>17</v>
       </c>
       <c r="O93" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="P93" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>601</v>
+        <v>385</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>17</v>
@@ -5614,13 +5615,13 @@
         <v>16</v>
       </c>
       <c r="M94" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N94" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O94" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P94" s="1" t="s">
         <v>17</v>
@@ -5628,16 +5629,16 @@
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>702</v>
+        <v>601</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>17</v>
@@ -5649,16 +5650,16 @@
         <v>17</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J95" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K95" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L95" s="1" t="s">
         <v>16</v>
@@ -5678,19 +5679,19 @@
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <v>483</v>
+        <v>702</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>17</v>
@@ -5699,16 +5700,22 @@
         <v>17</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J96" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="K96" s="1">
+        <v>3</v>
+      </c>
       <c r="L96" s="1" t="s">
         <v>16</v>
+      </c>
+      <c r="M96" s="1">
+        <v>1</v>
       </c>
       <c r="N96" s="1" t="s">
         <v>16</v>
@@ -5722,28 +5729,28 @@
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>502</v>
+        <v>483</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I97" s="1" t="s">
         <v>17</v>
@@ -5751,56 +5758,107 @@
       <c r="J97" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K97" s="1">
-        <v>1</v>
-      </c>
       <c r="L97" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="N97" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O97" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="P97" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="Q97" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
+        <v>502</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H98" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I98" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J98" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K98" s="1">
+        <v>1</v>
+      </c>
+      <c r="L98" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P98" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q98" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
         <v>213</v>
       </c>
-      <c r="B98" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F98" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G98" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H98" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I98" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J98" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L98" s="1" t="s">
+      <c r="B99" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H99" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I99" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J99" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L99" s="1" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A98" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{034a106e-6316-442c-ad35-738afd673d2b}" enabled="1" method="Standard" siteId="{cddc1229-ac2a-4b97-b78a-0e5cacb5865c}" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>